<commit_message>
Fixed Missing Points for Players
</commit_message>
<xml_diff>
--- a/Day 1 Results.xlsx
+++ b/Day 1 Results.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william.sampson/Documents/GitHub/InternationalFantasy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26BF65E5-CF43-0442-B8D7-743BE0A7E775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643E4B87-C3B7-C942-8FC6-95E44574A972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16820" yWindow="500" windowWidth="17540" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerSummary" sheetId="1" r:id="rId1"/>
     <sheet name="TeamSummary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="63">
   <si>
     <t>Participant</t>
   </si>
@@ -192,13 +205,31 @@
   </si>
   <si>
     <t>beastcoast</t>
+  </si>
+  <si>
+    <t>Topson</t>
+  </si>
+  <si>
+    <t>Nine</t>
+  </si>
+  <si>
+    <t>skiter</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Sneyking</t>
+  </si>
+  <si>
+    <t>Whitemon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +241,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -250,11 +288,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -598,7 +637,8 @@
         <v>566.33999999999992</v>
       </c>
       <c r="D2">
-        <v>1232.98</v>
+        <f>SUM(C2:C7)</f>
+        <v>1956.6599999999999</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -611,9 +651,6 @@
       <c r="C3">
         <v>342.54</v>
       </c>
-      <c r="D3">
-        <v>1232.98</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -623,10 +660,7 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>54</v>
-      </c>
-      <c r="D4">
-        <v>1232.98</v>
+        <v>260.82</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,55 +668,32 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C5">
-        <v>270.10000000000002</v>
-      </c>
-      <c r="D5">
-        <v>1232.98</v>
+        <v>294.58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="C6">
-        <v>332.49</v>
-      </c>
-      <c r="D6">
-        <v>868.05</v>
+        <v>222.28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>182.1</v>
-      </c>
-      <c r="D7">
-        <v>868.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>54</v>
-      </c>
-      <c r="D8">
-        <v>868.05</v>
+        <v>270.10000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -690,13 +701,14 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>73.819999999999993</v>
+        <v>332.49</v>
       </c>
       <c r="D9">
-        <v>868.05</v>
+        <f>SUM(C9:C14)</f>
+        <v>1177.0899999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -704,13 +716,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>107.58</v>
-      </c>
-      <c r="D10">
-        <v>868.05</v>
+        <v>182.1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -718,517 +727,674 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>118.06</v>
-      </c>
-      <c r="D11">
-        <v>868.05</v>
+        <v>260.82</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C12">
-        <v>81</v>
-      </c>
-      <c r="D12">
-        <v>130.02000000000001</v>
+        <v>176.04</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13">
-        <v>18.12</v>
-      </c>
-      <c r="D13">
-        <v>130.02000000000001</v>
+        <v>107.58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>30.9</v>
-      </c>
-      <c r="D14">
-        <v>130.02000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15">
-        <v>230.06</v>
-      </c>
-      <c r="D15">
-        <v>475.5</v>
+        <v>118.06</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>245.44</v>
+        <v>391.23</v>
       </c>
       <c r="D16">
-        <v>475.5</v>
+        <f>SUM(C16:C21)</f>
+        <v>1579.5699999999997</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C17">
-        <v>81</v>
-      </c>
-      <c r="D17">
-        <v>130.02000000000001</v>
+        <v>183.14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="C18">
-        <v>18.12</v>
-      </c>
-      <c r="D18">
-        <v>130.02000000000001</v>
+        <v>282.45999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="C19">
-        <v>30.9</v>
-      </c>
-      <c r="D19">
-        <v>130.02000000000001</v>
+        <v>294.58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C20">
-        <v>81</v>
-      </c>
-      <c r="D20">
-        <v>1136.8399999999999</v>
+        <v>222.28</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21">
-        <v>106.08</v>
-      </c>
-      <c r="D21">
-        <v>1136.8399999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22">
-        <v>377.55999999999989</v>
-      </c>
-      <c r="D22">
-        <v>1136.8399999999999</v>
+        <v>205.88</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C23">
-        <v>295.86</v>
+        <v>423.69000000000011</v>
       </c>
       <c r="D23">
-        <v>1136.8399999999999</v>
+        <f>SUM(C23:C28)</f>
+        <v>1744.5900000000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24">
-        <v>245.44</v>
-      </c>
-      <c r="D24">
-        <v>1136.8399999999999</v>
+        <v>230.06</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>30.9</v>
-      </c>
-      <c r="D25">
-        <v>1136.8399999999999</v>
+        <v>245.44</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C26">
-        <v>445.41</v>
-      </c>
-      <c r="D26">
-        <v>1172.95</v>
+        <v>294.58</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C27">
-        <v>54</v>
-      </c>
-      <c r="D27">
-        <v>1172.95</v>
+        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C28">
-        <v>295.86</v>
-      </c>
-      <c r="D28">
-        <v>1172.95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29">
-        <v>270.10000000000002</v>
-      </c>
-      <c r="D29">
-        <v>1172.95</v>
+        <v>307.82000000000011</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>107.58</v>
+        <v>391.23</v>
       </c>
       <c r="D30">
-        <v>1172.95</v>
+        <f>SUM(C30:C35)</f>
+        <v>1579.5699999999997</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>566.33999999999992</v>
-      </c>
-      <c r="D31">
-        <v>1232.98</v>
+        <v>183.14</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C32">
-        <v>342.54</v>
-      </c>
-      <c r="D32">
-        <v>1232.98</v>
+        <v>282.45999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C33">
-        <v>54</v>
-      </c>
-      <c r="D33">
-        <v>1232.98</v>
+        <v>294.58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C34">
-        <v>270.10000000000002</v>
-      </c>
-      <c r="D34">
-        <v>1232.98</v>
+        <v>222.28</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C35">
-        <v>81</v>
-      </c>
-      <c r="D35">
-        <v>1025.8599999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36">
-        <v>18.12</v>
-      </c>
-      <c r="D36">
-        <v>1025.8599999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37">
-        <v>33.64</v>
-      </c>
-      <c r="D37">
-        <v>1025.8599999999999</v>
+        <v>205.88</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C38">
-        <v>377.55999999999989</v>
+        <v>391.23</v>
       </c>
       <c r="D38">
-        <v>1025.8599999999999</v>
+        <f>SUM(C38:C43)</f>
+        <v>1741.15</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C39">
-        <v>270.10000000000002</v>
-      </c>
-      <c r="D39">
-        <v>1025.8599999999999</v>
+        <v>225.18</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C40">
-        <v>245.44</v>
-      </c>
-      <c r="D40">
-        <v>1025.8599999999999</v>
+        <v>377.55999999999989</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41">
-        <v>296.94</v>
-      </c>
-      <c r="D41">
-        <v>639.48</v>
+        <v>295.86</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C42">
-        <v>342.54</v>
-      </c>
-      <c r="D42">
-        <v>639.48</v>
+        <v>245.44</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C43">
-        <v>96.87</v>
-      </c>
-      <c r="D43">
-        <v>890.03</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44">
-        <v>71.739999999999995</v>
-      </c>
-      <c r="D44">
-        <v>890.03</v>
+        <v>205.88</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C45">
-        <v>236.28</v>
+        <v>445.41</v>
       </c>
       <c r="D45">
-        <v>890.03</v>
+        <f>SUM(C45:C50)</f>
+        <v>1601.4299999999998</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="C46">
-        <v>266.39999999999998</v>
-      </c>
-      <c r="D46">
-        <v>890.03</v>
+        <v>260.82</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47">
+        <v>221.66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48">
+        <v>295.86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49">
+        <v>270.10000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50">
+        <v>107.58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53">
+        <v>566.33999999999992</v>
+      </c>
+      <c r="D53">
+        <f>SUM(C53:C58)</f>
+        <v>1956.6599999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54">
+        <v>342.54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55">
+        <v>260.82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56">
+        <v>294.58</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57">
+        <v>222.28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58">
+        <v>270.10000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60">
+        <v>391.23</v>
+      </c>
+      <c r="D60">
+        <f>SUM(C60:C65)</f>
+        <v>1655.1100000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61">
+        <v>183.14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62">
+        <v>187.64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63">
+        <v>377.55999999999989</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64">
+        <v>270.10000000000002</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65">
+        <v>245.44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67">
+        <v>423.69000000000011</v>
+      </c>
+      <c r="D67">
+        <f>SUM(C67:C72)</f>
+        <v>1823.3300000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>13</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68">
+        <v>230.06</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69">
+        <v>296.94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70">
+        <v>342.54</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71">
+        <v>222.28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" t="s">
+        <v>61</v>
+      </c>
+      <c r="C72">
+        <v>307.82000000000011</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B74" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74">
+        <v>96.87</v>
+      </c>
+      <c r="D74">
+        <f>SUM(C74:C79)</f>
+        <v>1241.0700000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75">
+        <v>208.06</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76">
+        <v>236.28</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77">
+        <v>266.39999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="2">
+        <v>214.72</v>
+      </c>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" t="s">
         <v>36</v>
       </c>
-      <c r="C47">
+      <c r="C79">
         <v>218.74</v>
-      </c>
-      <c r="D47">
-        <v>890.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>